<commit_message>
Updated the Sample Template
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>Node Name</t>
   </si>
@@ -132,9 +132,6 @@
     <t>High Performance</t>
   </si>
   <si>
-    <t>Win2008 R2 Std 2 CPU</t>
-  </si>
-  <si>
     <t>Win2008 R2 Ent 2 CPU</t>
   </si>
   <si>
@@ -189,22 +186,13 @@
     <t>standard</t>
   </si>
   <si>
-    <t>Sample 01</t>
-  </si>
-  <si>
-    <t>172.26.0.11</t>
-  </si>
-  <si>
-    <t>Sample 02</t>
+    <t>Ubuntu 12.04 2 CPU</t>
   </si>
   <si>
     <t>172.26.0.12</t>
   </si>
   <si>
-    <t>Sample 03</t>
-  </si>
-  <si>
-    <t>172.26.0.13</t>
+    <t>Sample02</t>
   </si>
 </sst>
 </file>
@@ -539,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,10 +549,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
@@ -582,7 +570,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>8</v>
@@ -629,25 +617,25 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -656,131 +644,19 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2">
-        <v>200</v>
-      </c>
-      <c r="Q2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3">
-        <v>75</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3">
-        <v>50</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3">
-        <v>10</v>
-      </c>
-      <c r="S3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4">
-        <v>30</v>
-      </c>
-      <c r="O4" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -843,7 +719,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -873,7 +749,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -890,7 +766,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -904,7 +780,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
         <v>33</v>
@@ -912,47 +788,47 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>